<commit_message>
Uploaded updated test cases and acceptance criteria for scope of Sprint 8
</commit_message>
<xml_diff>
--- a/ProjectDocs/Artifacts/SymCheck Acceptance Criteria.xlsx
+++ b/ProjectDocs/Artifacts/SymCheck Acceptance Criteria.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://paceuniversity-my.sharepoint.com/personal/jw42299p_pace_edu/Documents/Spring2021/CS692/Sprint7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D5715382-F8C1-4883-A783-1527F3A581AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{CDC7B06E-EF96-4D9C-9278-736BBFD7C47D}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{D5715382-F8C1-4883-A783-1527F3A581AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4F29D9D-E40A-3C4C-9791-5B4D8B41D966}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{496174A1-1C1B-DD47-953B-A5A9CFC2B132}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{496174A1-1C1B-DD47-953B-A5A9CFC2B132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$22</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t>Acceptance Criteria</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>HID-62</t>
-  </si>
-  <si>
-    <t>1. Given that the patient has a browser open, when the patient types in SymCheck's URL, then the SymCheck application should be accessible without any errors.</t>
   </si>
   <si>
     <t>1. Given that the patient is on the ResultsPage, when the patient successfully submitted their image, then the ResultsPage should contain a seperate field that indicates under what conditions the patient should definitely see a doctor (i.e. age, state of pregnancy, etc.)</t>
@@ -216,6 +213,24 @@
   </si>
   <si>
     <t>Given that the patient is on the Homepage, when the user is reading the SymCheck info box, then the user.</t>
+  </si>
+  <si>
+    <t>Given that the patient opens a supported browser, when the patient navigates to www.symcheckapp.com, then the patient can utilize SymCheck</t>
+  </si>
+  <si>
+    <t>Given that the patient is on a mobile device using a supported browser, when the patient navigates to www.symcheckapp.com, then the patient will see a mobile friendly interface</t>
+  </si>
+  <si>
+    <t>MobileAcess</t>
+  </si>
+  <si>
+    <t>HID-64</t>
+  </si>
+  <si>
+    <t>HID-94</t>
+  </si>
+  <si>
+    <t>Given that the patient is on the Results page, when the patient receives a diagnosis, then the patient will see a progress bar showing their percentage</t>
   </si>
 </sst>
 </file>
@@ -694,23 +709,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="96.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="96.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="53.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -720,7 +735,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -737,24 +752,24 @@
       <c r="F2" s="3"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -771,15 +786,15 @@
       <c r="F4" s="3"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -788,83 +803,75 @@
       <c r="F5" s="3"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>38</v>
-      </c>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>1</v>
@@ -873,15 +880,15 @@
       <c r="F10" s="3"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>1</v>
@@ -890,49 +897,49 @@
       <c r="F11" s="3"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>3</v>
@@ -941,15 +948,15 @@
       <c r="F14" s="3"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -958,15 +965,15 @@
       <c r="F15" s="3"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>3</v>
@@ -975,15 +982,15 @@
       <c r="F16" s="3"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -992,110 +999,161 @@
       <c r="F17" s="3"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D24">
-    <sortCondition ref="D3:D24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D27">
+    <sortCondition ref="D3:D27"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -1107,12 +1165,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010004E81107FE0A704B8458C943278B4E1F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f5d7a2437a23173ad2037d1f1a5defc1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bcb18cd9-2614-41de-a438-05e8f58d2b4e" xmlns:ns4="9cd9834e-9656-4a9f-bc4d-b5b5e1a3e387" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="80d70d1cc08310b67696d51f78b76f76" ns3:_="" ns4:_="">
     <xsd:import namespace="bcb18cd9-2614-41de-a438-05e8f58d2b4e"/>
@@ -1323,6 +1375,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1333,23 +1391,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9973A34B-42BA-4BA6-8F6B-E8E99B4B3CE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bcb18cd9-2614-41de-a438-05e8f58d2b4e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9cd9834e-9656-4a9f-bc4d-b5b5e1a3e387"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{658742AD-23CF-459D-BF62-4769585AF84A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1368,6 +1409,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9973A34B-42BA-4BA6-8F6B-E8E99B4B3CE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bcb18cd9-2614-41de-a438-05e8f58d2b4e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9cd9834e-9656-4a9f-bc4d-b5b5e1a3e387"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF09264B-97F5-4B4A-88C6-C939F1F4B7CD}">
   <ds:schemaRefs>

</xml_diff>